<commit_message>
Slight update to algo logic -> MUCH better results
</commit_message>
<xml_diff>
--- a/schedule_input.xlsx
+++ b/schedule_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17300" yWindow="600" windowWidth="25980" windowHeight="21300" tabRatio="534"/>
+    <workbookView xWindow="9500" yWindow="900" windowWidth="25980" windowHeight="21300" tabRatio="534"/>
   </bookViews>
   <sheets>
     <sheet name="Recruit Preferences" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="96">
   <si>
     <t>Last Name</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Andrew</t>
   </si>
   <si>
-    <t>Hupp</t>
-  </si>
-  <si>
     <t>Professor Name</t>
   </si>
   <si>
@@ -307,6 +304,12 @@
   </si>
   <si>
     <t>Nano</t>
+  </si>
+  <si>
+    <t>Xie</t>
+  </si>
+  <si>
+    <t>Yushu</t>
   </si>
 </sst>
 </file>
@@ -1329,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMD26"/>
+  <dimension ref="A1:AMD27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1357,10 +1360,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -1380,16 +1383,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>15</v>
@@ -1403,10 +1406,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1426,10 +1429,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>8</v>
@@ -1449,10 +1452,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -1464,7 +1467,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
@@ -1472,10 +1475,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -1495,10 +1498,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -1518,10 +1521,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>8</v>
@@ -1541,10 +1544,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -1561,10 +1564,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>15</v>
@@ -1579,12 +1582,12 @@
         <v>3</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>21</v>
@@ -1607,10 +1610,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
@@ -1630,16 +1633,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -1648,15 +1651,15 @@
         <v>18</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>13</v>
@@ -1674,16 +1677,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>18</v>
@@ -1695,12 +1698,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:1018">
       <c r="A17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>11</v>
@@ -1709,7 +1712,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>8</v>
@@ -1718,12 +1721,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:1018">
       <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1741,12 +1744,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:1018">
       <c r="A19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
@@ -1764,12 +1767,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:1018">
       <c r="A20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
@@ -1787,15 +1790,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:1018">
       <c r="A21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>4</v>
@@ -1810,12 +1813,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:1018">
       <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -1833,12 +1836,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:1018">
       <c r="A23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>3</v>
@@ -1856,12 +1859,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:1018">
       <c r="A24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -1879,12 +1882,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:1018">
       <c r="A25" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>13</v>
@@ -1902,26 +1905,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:1018">
       <c r="A26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AMA26"/>
+      <c r="AMB26"/>
+      <c r="AMC26"/>
+      <c r="AMD26"/>
+    </row>
+    <row r="27" spans="1:1018">
+      <c r="A27" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="E27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G27" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1946,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK27"/>
+  <dimension ref="A1:AMK26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1960,28 +1990,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1989,27 +2019,27 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -2017,24 +2047,24 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2045,19 +2075,19 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2065,16 +2095,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -2082,10 +2112,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
@@ -2099,7 +2129,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="9"/>
@@ -2113,21 +2143,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="G9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="9"/>
@@ -2138,164 +2172,178 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="F12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>30</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="E14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="H15" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="F17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
@@ -2306,168 +2354,156 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="12"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="D21" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G21" s="11"/>
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="C23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E25" s="11"/>
       <c r="F25" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="F26" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2505,21 +2541,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="13">
         <v>6</v>
@@ -2575,33 +2611,33 @@
     <row r="1" spans="1:9" ht="13" thickBot="1">
       <c r="A1" s="19"/>
       <c r="B1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="E1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>40</v>
-      </c>
       <c r="G1" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="23">
         <v>0</v>
@@ -2630,7 +2666,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
@@ -2659,7 +2695,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="23">
         <v>3</v>
@@ -2688,7 +2724,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
@@ -2717,7 +2753,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="23">
         <v>5</v>
@@ -2746,7 +2782,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="17">
         <v>7</v>
@@ -2775,7 +2811,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="23">
         <v>4</v>
@@ -2804,7 +2840,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="17">
         <v>6</v>

</xml_diff>